<commit_message>
Add in other perturbations
</commit_message>
<xml_diff>
--- a/resources/manifests/1/manifest.example.xlsx
+++ b/resources/manifests/1/manifest.example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hjjoshi/dev/ms-checker/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hjjoshi/dev/ms-checker/resources/manifests/1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>auto</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>#Version</t>
+  </si>
+  <si>
+    <t>[Other Perturbations]</t>
+  </si>
+  <si>
+    <t>#Description</t>
   </si>
 </sst>
 </file>
@@ -545,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D22"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -727,6 +733,16 @@
         <v>15</v>
       </c>
     </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Read doi conf in from manifest
</commit_message>
<xml_diff>
--- a/resources/manifests/1/manifest.example.xlsx
+++ b/resources/manifests/1/manifest.example.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>auto</t>
   </si>
@@ -123,6 +123,15 @@
   </si>
   <si>
     <t>#Description</t>
+  </si>
+  <si>
+    <t>abc/def</t>
+  </si>
+  <si>
+    <t>[Publication]</t>
+  </si>
+  <si>
+    <t>#DOI</t>
   </si>
 </sst>
 </file>
@@ -551,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -743,6 +752,21 @@
         <v>32</v>
       </c>
     </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Add in quant conf and flag setting to manifests
</commit_message>
<xml_diff>
--- a/resources/manifests/1/manifest.example.xlsx
+++ b/resources/manifests/1/manifest.example.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="70880" yWindow="2840" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="81860" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>auto</t>
   </si>
@@ -132,6 +132,60 @@
   </si>
   <si>
     <t>#DOI</t>
+  </si>
+  <si>
+    <t>[Quantitation]</t>
+  </si>
+  <si>
+    <t>#Channel</t>
+  </si>
+  <si>
+    <t>#Identifier</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>wt</t>
+  </si>
+  <si>
+    <t>ko</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>sc</t>
+  </si>
+  <si>
+    <t>[Flags]</t>
+  </si>
+  <si>
+    <t>#Value</t>
+  </si>
+  <si>
+    <t>#Flag</t>
+  </si>
+  <si>
+    <t>hcd-alias</t>
+  </si>
+  <si>
+    <t>PQD</t>
+  </si>
+  <si>
+    <t>etd-alias</t>
+  </si>
+  <si>
+    <t>CID</t>
+  </si>
+  <si>
+    <t>feature_enable_truncated_nglyco</t>
+  </si>
+  <si>
+    <t>hcd-dont-use-masspeaks</t>
   </si>
 </sst>
 </file>
@@ -560,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -767,6 +821,88 @@
         <v>33</v>
       </c>
     </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>